<commit_message>
finish the main file
</commit_message>
<xml_diff>
--- a/Final/VQA Files/OurAnswers.xlsx
+++ b/Final/VQA Files/OurAnswers.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="309">
   <si>
     <t>Images</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>what shows l3 infectious spondylitis with bilateral psoas muscle abscess extension?</t>
-  </si>
-  <si>
-    <t>ct</t>
   </si>
   <si>
     <t>ymj-52-1044-g001</t>
@@ -1331,15 +1328,15 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1347,10 +1344,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1358,21 +1355,21 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1380,43 +1377,43 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1424,10 +1421,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1435,10 +1432,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1446,21 +1443,21 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1468,43 +1465,43 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
         <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1512,10 +1509,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
         <v>41</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -1523,21 +1520,21 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
         <v>45</v>
-      </c>
-      <c r="B22" t="s">
-        <v>46</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1545,32 +1542,32 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
         <v>49</v>
       </c>
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
         <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -1578,10 +1575,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
         <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -1589,21 +1586,21 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
         <v>55</v>
       </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
         <v>57</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1611,21 +1608,21 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
         <v>59</v>
       </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
         <v>61</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -1633,32 +1630,32 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
         <v>63</v>
       </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
         <v>65</v>
       </c>
-      <c r="B32" t="s">
-        <v>66</v>
-      </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
         <v>67</v>
-      </c>
-      <c r="B33" t="s">
-        <v>68</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1666,10 +1663,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" t="s">
         <v>69</v>
-      </c>
-      <c r="B34" t="s">
-        <v>70</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -1677,21 +1674,21 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
         <v>71</v>
       </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
         <v>73</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -1699,10 +1696,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
         <v>75</v>
-      </c>
-      <c r="B37" t="s">
-        <v>76</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -1710,43 +1707,43 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
         <v>77</v>
       </c>
-      <c r="B38" t="s">
-        <v>78</v>
-      </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
         <v>79</v>
       </c>
-      <c r="B39" t="s">
-        <v>80</v>
-      </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
         <v>81</v>
       </c>
-      <c r="B40" t="s">
-        <v>82</v>
-      </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
         <v>83</v>
-      </c>
-      <c r="B41" t="s">
-        <v>84</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -1754,10 +1751,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
         <v>85</v>
-      </c>
-      <c r="B42" t="s">
-        <v>86</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -1765,10 +1762,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
         <v>87</v>
-      </c>
-      <c r="B43" t="s">
-        <v>88</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -1776,21 +1773,21 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
         <v>89</v>
       </c>
-      <c r="B44" t="s">
-        <v>90</v>
-      </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
         <v>91</v>
-      </c>
-      <c r="B45" t="s">
-        <v>92</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1798,10 +1795,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
         <v>93</v>
-      </c>
-      <c r="B46" t="s">
-        <v>94</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1809,10 +1806,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
         <v>95</v>
-      </c>
-      <c r="B47" t="s">
-        <v>96</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1820,21 +1817,21 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
         <v>97</v>
       </c>
-      <c r="B48" t="s">
-        <v>98</v>
-      </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
         <v>99</v>
-      </c>
-      <c r="B49" t="s">
-        <v>100</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1842,21 +1839,21 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
         <v>101</v>
       </c>
-      <c r="B50" t="s">
-        <v>102</v>
-      </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
         <v>103</v>
-      </c>
-      <c r="B51" t="s">
-        <v>104</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1864,10 +1861,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" t="s">
         <v>105</v>
-      </c>
-      <c r="B52" t="s">
-        <v>106</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -1875,10 +1872,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" t="s">
         <v>107</v>
-      </c>
-      <c r="B53" t="s">
-        <v>108</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1886,21 +1883,21 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
         <v>109</v>
       </c>
-      <c r="B54" t="s">
-        <v>110</v>
-      </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" t="s">
         <v>111</v>
-      </c>
-      <c r="B55" t="s">
-        <v>112</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -1908,21 +1905,21 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" t="s">
         <v>113</v>
       </c>
-      <c r="B56" t="s">
-        <v>114</v>
-      </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" t="s">
         <v>115</v>
-      </c>
-      <c r="B57" t="s">
-        <v>116</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1930,10 +1927,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
         <v>117</v>
-      </c>
-      <c r="B58" t="s">
-        <v>118</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -1941,10 +1938,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" t="s">
         <v>119</v>
-      </c>
-      <c r="B59" t="s">
-        <v>120</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1952,10 +1949,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
         <v>121</v>
-      </c>
-      <c r="B60" t="s">
-        <v>122</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -1963,21 +1960,21 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" t="s">
         <v>123</v>
       </c>
-      <c r="B61" t="s">
-        <v>124</v>
-      </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" t="s">
         <v>125</v>
-      </c>
-      <c r="B62" t="s">
-        <v>126</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1985,10 +1982,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
         <v>127</v>
-      </c>
-      <c r="B63" t="s">
-        <v>128</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -1996,10 +1993,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" t="s">
         <v>129</v>
-      </c>
-      <c r="B64" t="s">
-        <v>130</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -2007,10 +2004,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" t="s">
         <v>131</v>
-      </c>
-      <c r="B65" t="s">
-        <v>132</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
@@ -2018,10 +2015,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" t="s">
         <v>133</v>
-      </c>
-      <c r="B66" t="s">
-        <v>134</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
@@ -2029,21 +2026,21 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" t="s">
         <v>135</v>
       </c>
-      <c r="B67" t="s">
-        <v>136</v>
-      </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
         <v>137</v>
-      </c>
-      <c r="B68" t="s">
-        <v>138</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -2051,21 +2048,21 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
         <v>139</v>
       </c>
-      <c r="B69" t="s">
-        <v>140</v>
-      </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" t="s">
         <v>141</v>
-      </c>
-      <c r="B70" t="s">
-        <v>142</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -2073,21 +2070,21 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
         <v>143</v>
       </c>
-      <c r="B71" t="s">
-        <v>144</v>
-      </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" t="s">
         <v>145</v>
-      </c>
-      <c r="B72" t="s">
-        <v>146</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
@@ -2095,21 +2092,21 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" t="s">
         <v>147</v>
       </c>
-      <c r="B73" t="s">
-        <v>148</v>
-      </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" t="s">
         <v>149</v>
-      </c>
-      <c r="B74" t="s">
-        <v>150</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
@@ -2117,10 +2114,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" t="s">
         <v>151</v>
-      </c>
-      <c r="B75" t="s">
-        <v>152</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
@@ -2128,43 +2125,43 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
         <v>153</v>
       </c>
-      <c r="B76" t="s">
-        <v>154</v>
-      </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
         <v>155</v>
       </c>
-      <c r="B77" t="s">
-        <v>156</v>
-      </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
+        <v>156</v>
+      </c>
+      <c r="B78" t="s">
         <v>157</v>
       </c>
-      <c r="B78" t="s">
-        <v>158</v>
-      </c>
       <c r="C78" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
+        <v>158</v>
+      </c>
+      <c r="B79" t="s">
         <v>159</v>
-      </c>
-      <c r="B79" t="s">
-        <v>160</v>
       </c>
       <c r="C79" t="s">
         <v>5</v>
@@ -2172,32 +2169,32 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
+        <v>160</v>
+      </c>
+      <c r="B80" t="s">
         <v>161</v>
       </c>
-      <c r="B80" t="s">
-        <v>162</v>
-      </c>
       <c r="C80" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
+        <v>162</v>
+      </c>
+      <c r="B81" t="s">
         <v>163</v>
       </c>
-      <c r="B81" t="s">
-        <v>164</v>
-      </c>
       <c r="C81" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
+        <v>164</v>
+      </c>
+      <c r="B82" t="s">
         <v>165</v>
-      </c>
-      <c r="B82" t="s">
-        <v>166</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
@@ -2205,21 +2202,21 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
+        <v>166</v>
+      </c>
+      <c r="B83" t="s">
         <v>167</v>
       </c>
-      <c r="B83" t="s">
-        <v>168</v>
-      </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84" t="s">
         <v>169</v>
-      </c>
-      <c r="B84" t="s">
-        <v>170</v>
       </c>
       <c r="C84" t="s">
         <v>5</v>
@@ -2227,32 +2224,32 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" t="s">
         <v>171</v>
       </c>
-      <c r="B85" t="s">
-        <v>172</v>
-      </c>
       <c r="C85" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
+        <v>172</v>
+      </c>
+      <c r="B86" t="s">
         <v>173</v>
       </c>
-      <c r="B86" t="s">
-        <v>174</v>
-      </c>
       <c r="C86" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
+        <v>174</v>
+      </c>
+      <c r="B87" t="s">
         <v>175</v>
-      </c>
-      <c r="B87" t="s">
-        <v>176</v>
       </c>
       <c r="C87" t="s">
         <v>5</v>
@@ -2260,10 +2257,10 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" t="s">
         <v>177</v>
-      </c>
-      <c r="B88" t="s">
-        <v>178</v>
       </c>
       <c r="C88" t="s">
         <v>5</v>
@@ -2271,10 +2268,10 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
+        <v>178</v>
+      </c>
+      <c r="B89" t="s">
         <v>179</v>
-      </c>
-      <c r="B89" t="s">
-        <v>180</v>
       </c>
       <c r="C89" t="s">
         <v>5</v>
@@ -2282,10 +2279,10 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
+        <v>180</v>
+      </c>
+      <c r="B90" t="s">
         <v>181</v>
-      </c>
-      <c r="B90" t="s">
-        <v>182</v>
       </c>
       <c r="C90" t="s">
         <v>5</v>
@@ -2293,10 +2290,10 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" t="s">
         <v>183</v>
-      </c>
-      <c r="B91" t="s">
-        <v>184</v>
       </c>
       <c r="C91" t="s">
         <v>5</v>
@@ -2304,10 +2301,10 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>184</v>
+      </c>
+      <c r="B92" t="s">
         <v>185</v>
-      </c>
-      <c r="B92" t="s">
-        <v>186</v>
       </c>
       <c r="C92" t="s">
         <v>5</v>
@@ -2315,10 +2312,10 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
+        <v>186</v>
+      </c>
+      <c r="B93" t="s">
         <v>187</v>
-      </c>
-      <c r="B93" t="s">
-        <v>188</v>
       </c>
       <c r="C93" t="s">
         <v>5</v>
@@ -2326,10 +2323,10 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
+        <v>188</v>
+      </c>
+      <c r="B94" t="s">
         <v>189</v>
-      </c>
-      <c r="B94" t="s">
-        <v>190</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
@@ -2337,10 +2334,10 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" t="s">
         <v>191</v>
-      </c>
-      <c r="B95" t="s">
-        <v>192</v>
       </c>
       <c r="C95" t="s">
         <v>5</v>
@@ -2348,10 +2345,10 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
+        <v>192</v>
+      </c>
+      <c r="B96" t="s">
         <v>193</v>
-      </c>
-      <c r="B96" t="s">
-        <v>194</v>
       </c>
       <c r="C96" t="s">
         <v>5</v>
@@ -2359,10 +2356,10 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
+        <v>194</v>
+      </c>
+      <c r="B97" t="s">
         <v>195</v>
-      </c>
-      <c r="B97" t="s">
-        <v>196</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
@@ -2370,10 +2367,10 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
+        <v>196</v>
+      </c>
+      <c r="B98" t="s">
         <v>197</v>
-      </c>
-      <c r="B98" t="s">
-        <v>198</v>
       </c>
       <c r="C98" t="s">
         <v>5</v>
@@ -2381,10 +2378,10 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
+        <v>198</v>
+      </c>
+      <c r="B99" t="s">
         <v>199</v>
-      </c>
-      <c r="B99" t="s">
-        <v>200</v>
       </c>
       <c r="C99" t="s">
         <v>5</v>
@@ -2392,10 +2389,10 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
+        <v>200</v>
+      </c>
+      <c r="B100" t="s">
         <v>201</v>
-      </c>
-      <c r="B100" t="s">
-        <v>202</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>
@@ -2403,21 +2400,21 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
+        <v>202</v>
+      </c>
+      <c r="B101" t="s">
         <v>203</v>
       </c>
-      <c r="B101" t="s">
-        <v>204</v>
-      </c>
       <c r="C101" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
+        <v>204</v>
+      </c>
+      <c r="B102" t="s">
         <v>205</v>
-      </c>
-      <c r="B102" t="s">
-        <v>206</v>
       </c>
       <c r="C102" t="s">
         <v>5</v>
@@ -2425,10 +2422,10 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
+        <v>206</v>
+      </c>
+      <c r="B103" t="s">
         <v>207</v>
-      </c>
-      <c r="B103" t="s">
-        <v>208</v>
       </c>
       <c r="C103" t="s">
         <v>5</v>
@@ -2436,10 +2433,10 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
+        <v>208</v>
+      </c>
+      <c r="B104" t="s">
         <v>209</v>
-      </c>
-      <c r="B104" t="s">
-        <v>210</v>
       </c>
       <c r="C104" t="s">
         <v>5</v>
@@ -2447,10 +2444,10 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
+        <v>210</v>
+      </c>
+      <c r="B105" t="s">
         <v>211</v>
-      </c>
-      <c r="B105" t="s">
-        <v>212</v>
       </c>
       <c r="C105" t="s">
         <v>5</v>
@@ -2458,10 +2455,10 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B106" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C106" t="s">
         <v>5</v>
@@ -2469,21 +2466,21 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
+        <v>213</v>
+      </c>
+      <c r="B107" t="s">
         <v>214</v>
       </c>
-      <c r="B107" t="s">
-        <v>215</v>
-      </c>
       <c r="C107" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
+        <v>215</v>
+      </c>
+      <c r="B108" t="s">
         <v>216</v>
-      </c>
-      <c r="B108" t="s">
-        <v>217</v>
       </c>
       <c r="C108" t="s">
         <v>5</v>
@@ -2491,10 +2488,10 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
+        <v>217</v>
+      </c>
+      <c r="B109" t="s">
         <v>218</v>
-      </c>
-      <c r="B109" t="s">
-        <v>219</v>
       </c>
       <c r="C109" t="s">
         <v>5</v>
@@ -2502,21 +2499,21 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
+        <v>219</v>
+      </c>
+      <c r="B110" t="s">
         <v>220</v>
       </c>
-      <c r="B110" t="s">
-        <v>221</v>
-      </c>
       <c r="C110" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
+        <v>221</v>
+      </c>
+      <c r="B111" t="s">
         <v>222</v>
-      </c>
-      <c r="B111" t="s">
-        <v>223</v>
       </c>
       <c r="C111" t="s">
         <v>5</v>
@@ -2524,10 +2521,10 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
+        <v>223</v>
+      </c>
+      <c r="B112" t="s">
         <v>224</v>
-      </c>
-      <c r="B112" t="s">
-        <v>225</v>
       </c>
       <c r="C112" t="s">
         <v>5</v>
@@ -2535,21 +2532,21 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
+        <v>225</v>
+      </c>
+      <c r="B113" t="s">
         <v>226</v>
       </c>
-      <c r="B113" t="s">
-        <v>227</v>
-      </c>
       <c r="C113" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
+        <v>227</v>
+      </c>
+      <c r="B114" t="s">
         <v>228</v>
-      </c>
-      <c r="B114" t="s">
-        <v>229</v>
       </c>
       <c r="C114" t="s">
         <v>5</v>
@@ -2557,10 +2554,10 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
+        <v>229</v>
+      </c>
+      <c r="B115" t="s">
         <v>230</v>
-      </c>
-      <c r="B115" t="s">
-        <v>231</v>
       </c>
       <c r="C115" t="s">
         <v>5</v>
@@ -2568,10 +2565,10 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
+        <v>231</v>
+      </c>
+      <c r="B116" t="s">
         <v>232</v>
-      </c>
-      <c r="B116" t="s">
-        <v>233</v>
       </c>
       <c r="C116" t="s">
         <v>5</v>
@@ -2579,32 +2576,32 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
+        <v>233</v>
+      </c>
+      <c r="B117" t="s">
         <v>234</v>
       </c>
-      <c r="B117" t="s">
-        <v>235</v>
-      </c>
       <c r="C117" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
+        <v>235</v>
+      </c>
+      <c r="B118" t="s">
         <v>236</v>
       </c>
-      <c r="B118" t="s">
-        <v>237</v>
-      </c>
       <c r="C118" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
+        <v>237</v>
+      </c>
+      <c r="B119" t="s">
         <v>238</v>
-      </c>
-      <c r="B119" t="s">
-        <v>239</v>
       </c>
       <c r="C119" t="s">
         <v>5</v>
@@ -2612,10 +2609,10 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
+        <v>239</v>
+      </c>
+      <c r="B120" t="s">
         <v>240</v>
-      </c>
-      <c r="B120" t="s">
-        <v>241</v>
       </c>
       <c r="C120" t="s">
         <v>5</v>
@@ -2623,21 +2620,21 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
+        <v>241</v>
+      </c>
+      <c r="B121" t="s">
         <v>242</v>
       </c>
-      <c r="B121" t="s">
-        <v>243</v>
-      </c>
       <c r="C121" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
+        <v>243</v>
+      </c>
+      <c r="B122" t="s">
         <v>244</v>
-      </c>
-      <c r="B122" t="s">
-        <v>245</v>
       </c>
       <c r="C122" t="s">
         <v>5</v>
@@ -2645,10 +2642,10 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
+        <v>245</v>
+      </c>
+      <c r="B123" t="s">
         <v>246</v>
-      </c>
-      <c r="B123" t="s">
-        <v>247</v>
       </c>
       <c r="C123" t="s">
         <v>5</v>
@@ -2656,32 +2653,32 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
+        <v>247</v>
+      </c>
+      <c r="B124" t="s">
         <v>248</v>
       </c>
-      <c r="B124" t="s">
-        <v>249</v>
-      </c>
       <c r="C124" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
+        <v>249</v>
+      </c>
+      <c r="B125" t="s">
         <v>250</v>
       </c>
-      <c r="B125" t="s">
-        <v>251</v>
-      </c>
       <c r="C125" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
+        <v>251</v>
+      </c>
+      <c r="B126" t="s">
         <v>252</v>
-      </c>
-      <c r="B126" t="s">
-        <v>253</v>
       </c>
       <c r="C126" t="s">
         <v>5</v>
@@ -2689,54 +2686,54 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
+        <v>253</v>
+      </c>
+      <c r="B127" t="s">
         <v>254</v>
       </c>
-      <c r="B127" t="s">
-        <v>255</v>
-      </c>
       <c r="C127" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
+        <v>255</v>
+      </c>
+      <c r="B128" t="s">
         <v>256</v>
       </c>
-      <c r="B128" t="s">
-        <v>257</v>
-      </c>
       <c r="C128" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
+        <v>257</v>
+      </c>
+      <c r="B129" t="s">
         <v>258</v>
       </c>
-      <c r="B129" t="s">
-        <v>259</v>
-      </c>
       <c r="C129" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
+        <v>259</v>
+      </c>
+      <c r="B130" t="s">
         <v>260</v>
       </c>
-      <c r="B130" t="s">
-        <v>261</v>
-      </c>
       <c r="C130" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
+        <v>261</v>
+      </c>
+      <c r="B131" t="s">
         <v>262</v>
-      </c>
-      <c r="B131" t="s">
-        <v>263</v>
       </c>
       <c r="C131" t="s">
         <v>5</v>
@@ -2744,10 +2741,10 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
+        <v>263</v>
+      </c>
+      <c r="B132" t="s">
         <v>264</v>
-      </c>
-      <c r="B132" t="s">
-        <v>265</v>
       </c>
       <c r="C132" t="s">
         <v>5</v>
@@ -2755,10 +2752,10 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
+        <v>265</v>
+      </c>
+      <c r="B133" t="s">
         <v>266</v>
-      </c>
-      <c r="B133" t="s">
-        <v>267</v>
       </c>
       <c r="C133" t="s">
         <v>5</v>
@@ -2766,10 +2763,10 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
+        <v>267</v>
+      </c>
+      <c r="B134" t="s">
         <v>268</v>
-      </c>
-      <c r="B134" t="s">
-        <v>269</v>
       </c>
       <c r="C134" t="s">
         <v>5</v>
@@ -2777,10 +2774,10 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
+        <v>269</v>
+      </c>
+      <c r="B135" t="s">
         <v>270</v>
-      </c>
-      <c r="B135" t="s">
-        <v>271</v>
       </c>
       <c r="C135" t="s">
         <v>5</v>
@@ -2788,76 +2785,76 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
+        <v>271</v>
+      </c>
+      <c r="B136" t="s">
         <v>272</v>
       </c>
-      <c r="B136" t="s">
-        <v>273</v>
-      </c>
       <c r="C136" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
+        <v>273</v>
+      </c>
+      <c r="B137" t="s">
         <v>274</v>
       </c>
-      <c r="B137" t="s">
-        <v>275</v>
-      </c>
       <c r="C137" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
+        <v>275</v>
+      </c>
+      <c r="B138" t="s">
         <v>276</v>
       </c>
-      <c r="B138" t="s">
-        <v>277</v>
-      </c>
       <c r="C138" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
+        <v>277</v>
+      </c>
+      <c r="B139" t="s">
         <v>278</v>
       </c>
-      <c r="B139" t="s">
-        <v>279</v>
-      </c>
       <c r="C139" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
+        <v>279</v>
+      </c>
+      <c r="B140" t="s">
         <v>280</v>
       </c>
-      <c r="B140" t="s">
-        <v>281</v>
-      </c>
       <c r="C140" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
+        <v>281</v>
+      </c>
+      <c r="B141" t="s">
         <v>282</v>
       </c>
-      <c r="B141" t="s">
-        <v>283</v>
-      </c>
       <c r="C141" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
+        <v>283</v>
+      </c>
+      <c r="B142" t="s">
         <v>284</v>
-      </c>
-      <c r="B142" t="s">
-        <v>285</v>
       </c>
       <c r="C142" t="s">
         <v>5</v>
@@ -2865,21 +2862,21 @@
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
+        <v>285</v>
+      </c>
+      <c r="B143" t="s">
         <v>286</v>
       </c>
-      <c r="B143" t="s">
-        <v>287</v>
-      </c>
       <c r="C143" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
+        <v>287</v>
+      </c>
+      <c r="B144" t="s">
         <v>288</v>
-      </c>
-      <c r="B144" t="s">
-        <v>289</v>
       </c>
       <c r="C144" t="s">
         <v>5</v>
@@ -2887,10 +2884,10 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
+        <v>289</v>
+      </c>
+      <c r="B145" t="s">
         <v>290</v>
-      </c>
-      <c r="B145" t="s">
-        <v>291</v>
       </c>
       <c r="C145" t="s">
         <v>5</v>
@@ -2898,21 +2895,21 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
+        <v>291</v>
+      </c>
+      <c r="B146" t="s">
         <v>292</v>
       </c>
-      <c r="B146" t="s">
-        <v>293</v>
-      </c>
       <c r="C146" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
+        <v>293</v>
+      </c>
+      <c r="B147" t="s">
         <v>294</v>
-      </c>
-      <c r="B147" t="s">
-        <v>295</v>
       </c>
       <c r="C147" t="s">
         <v>5</v>
@@ -2920,21 +2917,21 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
+        <v>295</v>
+      </c>
+      <c r="B148" t="s">
         <v>296</v>
       </c>
-      <c r="B148" t="s">
-        <v>297</v>
-      </c>
       <c r="C148" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
+        <v>297</v>
+      </c>
+      <c r="B149" t="s">
         <v>298</v>
-      </c>
-      <c r="B149" t="s">
-        <v>299</v>
       </c>
       <c r="C149" t="s">
         <v>5</v>
@@ -2942,10 +2939,10 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
+        <v>299</v>
+      </c>
+      <c r="B150" t="s">
         <v>300</v>
-      </c>
-      <c r="B150" t="s">
-        <v>301</v>
       </c>
       <c r="C150" t="s">
         <v>5</v>
@@ -2953,32 +2950,32 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
+        <v>301</v>
+      </c>
+      <c r="B151" t="s">
         <v>302</v>
       </c>
-      <c r="B151" t="s">
-        <v>303</v>
-      </c>
       <c r="C151" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
+        <v>303</v>
+      </c>
+      <c r="B152" t="s">
         <v>304</v>
       </c>
-      <c r="B152" t="s">
-        <v>305</v>
-      </c>
       <c r="C152" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
+        <v>305</v>
+      </c>
+      <c r="B153" t="s">
         <v>306</v>
-      </c>
-      <c r="B153" t="s">
-        <v>307</v>
       </c>
       <c r="C153" t="s">
         <v>5</v>
@@ -2986,10 +2983,10 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
+        <v>307</v>
+      </c>
+      <c r="B154" t="s">
         <v>308</v>
-      </c>
-      <c r="B154" t="s">
-        <v>309</v>
       </c>
       <c r="C154" t="s">
         <v>5</v>

</xml_diff>